<commit_message>
Day11 - Citizenship with Apache POI
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/Resources/ScenarioResults.xlsx
+++ b/src/test/java/ApachePOI/Resources/ScenarioResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>68691a11-f529-4da6-8251-5bfd4e23d73d</t>
   </si>
@@ -93,6 +93,33 @@
   </si>
   <si>
     <t>PT8.8243856S</t>
+  </si>
+  <si>
+    <t>5a589b69-5978-4b07-9c29-72ffd3469ef7</t>
+  </si>
+  <si>
+    <t>Create Citizenship by getting data from Excel</t>
+  </si>
+  <si>
+    <t>2023-10-03T19:28:47.313812</t>
+  </si>
+  <si>
+    <t>2023-10-03T19:28:58.174485900</t>
+  </si>
+  <si>
+    <t>PT10.8606739S</t>
+  </si>
+  <si>
+    <t>9e6d51ca-1be3-4fff-b576-811a84b9476c</t>
+  </si>
+  <si>
+    <t>2023-10-03T19:33:51.493257200</t>
+  </si>
+  <si>
+    <t>2023-10-03T19:34:15.462612400</t>
+  </si>
+  <si>
+    <t>PT23.9693552S</t>
   </si>
 </sst>
 </file>
@@ -137,7 +164,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -243,6 +270,46 @@
         <v>26</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
JDBC - Day 01
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/Resources/ScenarioResults.xlsx
+++ b/src/test/java/ApachePOI/Resources/ScenarioResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>68691a11-f529-4da6-8251-5bfd4e23d73d</t>
   </si>
@@ -120,6 +120,18 @@
   </si>
   <si>
     <t>PT23.9693552S</t>
+  </si>
+  <si>
+    <t>84ec514e-b81d-4773-8859-f85d7adf8d5d</t>
+  </si>
+  <si>
+    <t>2023-10-05T03:08:46.196461</t>
+  </si>
+  <si>
+    <t>2023-10-05T03:09:01.847120500</t>
+  </si>
+  <si>
+    <t>PT15.6506595S</t>
   </si>
 </sst>
 </file>
@@ -164,7 +176,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -310,6 +322,26 @@
         <v>35</v>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
JDBC - Day 02
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/Resources/ScenarioResults.xlsx
+++ b/src/test/java/ApachePOI/Resources/ScenarioResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>68691a11-f529-4da6-8251-5bfd4e23d73d</t>
   </si>
@@ -132,6 +132,33 @@
   </si>
   <si>
     <t>PT15.6506595S</t>
+  </si>
+  <si>
+    <t>9dc456b6-fdde-4436-b439-8c4c08021251</t>
+  </si>
+  <si>
+    <t>Check if the data is correct</t>
+  </si>
+  <si>
+    <t>2023-10-17T20:36:24.589202300</t>
+  </si>
+  <si>
+    <t>2023-10-17T20:36:36.957066300</t>
+  </si>
+  <si>
+    <t>PT12.367864S</t>
+  </si>
+  <si>
+    <t>5ba4aee7-d573-4eca-a329-363b270ef726</t>
+  </si>
+  <si>
+    <t>2023-10-17T20:37:09.512879300</t>
+  </si>
+  <si>
+    <t>2023-10-17T20:37:17.579851900</t>
+  </si>
+  <si>
+    <t>PT8.0669726S</t>
   </si>
 </sst>
 </file>
@@ -176,7 +203,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -342,6 +369,46 @@
         <v>39</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s" s="0">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Rest Assured - Campus Country API Test
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/Resources/ScenarioResults.xlsx
+++ b/src/test/java/ApachePOI/Resources/ScenarioResults.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
   <si>
     <t>68691a11-f529-4da6-8251-5bfd4e23d73d</t>
   </si>
@@ -159,6 +159,54 @@
   </si>
   <si>
     <t>PT8.0669726S</t>
+  </si>
+  <si>
+    <t>1ecf9b45-3cb4-44f7-8406-405330071b14</t>
+  </si>
+  <si>
+    <t>2023-10-18T14:51:44.079540800</t>
+  </si>
+  <si>
+    <t>2023-10-18T14:51:49.382178900</t>
+  </si>
+  <si>
+    <t>PT5.3026381S</t>
+  </si>
+  <si>
+    <t>340a6953-2cd7-4db1-bfd6-65c534d290a4</t>
+  </si>
+  <si>
+    <t>2023-10-18T14:52:45.036011200</t>
+  </si>
+  <si>
+    <t>2023-10-18T14:52:49.303162200</t>
+  </si>
+  <si>
+    <t>PT4.267151S</t>
+  </si>
+  <si>
+    <t>adf5a47e-f644-4519-8965-263608b3af15</t>
+  </si>
+  <si>
+    <t>2023-10-18T14:53:42.420576</t>
+  </si>
+  <si>
+    <t>2023-10-18T14:53:47.147197900</t>
+  </si>
+  <si>
+    <t>PT4.7266219S</t>
+  </si>
+  <si>
+    <t>e68beea1-1508-45de-a585-6239a4beb37b</t>
+  </si>
+  <si>
+    <t>2023-10-18T14:54:40.656899600</t>
+  </si>
+  <si>
+    <t>2023-10-18T14:54:48.843654200</t>
+  </si>
+  <si>
+    <t>PT8.1867546S</t>
   </si>
 </sst>
 </file>
@@ -203,7 +251,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -409,6 +457,86 @@
         <v>48</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="E12" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="F12" t="s" s="0">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="F13" t="s" s="0">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="E14" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="F14" t="s" s="0">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>